<commit_message>
Add area renaming for bdi/ben_survey
</commit_message>
<xml_diff>
--- a/data/hivdata_survey_datasets.xlsx
+++ b/data/hivdata_survey_datasets.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11790" uniqueCount="903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11799" uniqueCount="908">
   <si>
     <t>Tables reflect analysis ready datasets. Non-analytical values (don't know, missing) are recoded as NA.</t>
   </si>
@@ -2426,6 +2426,9 @@
     <t>Oueme</t>
   </si>
   <si>
+    <t>Ouã©Mã©</t>
+  </si>
+  <si>
     <t>Mzuzu city</t>
   </si>
   <si>
@@ -2793,6 +2796,18 @@
   </si>
   <si>
     <t>Haut-Mbomou</t>
+  </si>
+  <si>
+    <t>Karusi</t>
+  </si>
+  <si>
+    <t>Karuzi</t>
+  </si>
+  <si>
+    <t>Bururi Rural</t>
+  </si>
+  <si>
+    <t>Bururi</t>
   </si>
 </sst>
 </file>
@@ -3954,12 +3969,12 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D150"/>
+  <dimension ref="A1:D153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B148" sqref="B148"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="$A21:$XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="3"/>
@@ -4200,7 +4215,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" customFormat="1" spans="1:3">
       <c r="A20" t="s">
         <v>527</v>
       </c>
@@ -4211,29 +4226,29 @@
         <v>779</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>406</v>
-      </c>
-      <c r="B21" t="s">
+    <row r="21" s="1" customFormat="1" spans="1:3">
+      <c r="A21" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>780</v>
       </c>
-      <c r="C21" t="s">
-        <v>781</v>
-      </c>
-      <c r="D21" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="C21" s="1" t="s">
+        <v>779</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>406</v>
       </c>
       <c r="B22" t="s">
+        <v>781</v>
+      </c>
+      <c r="C22" t="s">
+        <v>782</v>
+      </c>
+      <c r="D22" t="s">
         <v>783</v>
-      </c>
-      <c r="C22" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -4241,10 +4256,10 @@
         <v>406</v>
       </c>
       <c r="B23" t="s">
+        <v>784</v>
+      </c>
+      <c r="C23" t="s">
         <v>785</v>
-      </c>
-      <c r="C23" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -4252,35 +4267,35 @@
         <v>406</v>
       </c>
       <c r="B24" t="s">
+        <v>786</v>
+      </c>
+      <c r="C24" t="s">
         <v>787</v>
       </c>
-      <c r="C24" t="s">
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>406</v>
+      </c>
+      <c r="B25" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="25" customFormat="1" spans="1:4">
-      <c r="A25" t="s">
-        <v>520</v>
-      </c>
-      <c r="B25" t="s">
-        <v>780</v>
-      </c>
       <c r="C25" t="s">
-        <v>781</v>
-      </c>
-      <c r="D25" t="s">
-        <v>782</v>
-      </c>
-    </row>
-    <row r="26" customFormat="1" spans="1:3">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="26" customFormat="1" spans="1:4">
       <c r="A26" t="s">
         <v>520</v>
       </c>
       <c r="B26" t="s">
+        <v>781</v>
+      </c>
+      <c r="C26" t="s">
+        <v>782</v>
+      </c>
+      <c r="D26" t="s">
         <v>783</v>
-      </c>
-      <c r="C26" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="27" customFormat="1" spans="1:3">
@@ -4288,10 +4303,10 @@
         <v>520</v>
       </c>
       <c r="B27" t="s">
+        <v>784</v>
+      </c>
+      <c r="C27" t="s">
         <v>785</v>
-      </c>
-      <c r="C27" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="28" customFormat="1" spans="1:3">
@@ -4299,21 +4314,21 @@
         <v>520</v>
       </c>
       <c r="B28" t="s">
+        <v>786</v>
+      </c>
+      <c r="C28" t="s">
         <v>787</v>
       </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="29" customFormat="1" spans="1:3">
+      <c r="A29" t="s">
+        <v>520</v>
+      </c>
+      <c r="B29" t="s">
         <v>788</v>
       </c>
-    </row>
-    <row r="29" s="1" customFormat="1" spans="1:3">
-      <c r="A29" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" t="s">
         <v>789</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>790</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="1" spans="1:3">
@@ -4321,10 +4336,10 @@
         <v>534</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>791</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="1" spans="1:3">
@@ -4332,10 +4347,10 @@
         <v>534</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>793</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>794</v>
       </c>
     </row>
     <row r="32" s="1" customFormat="1" spans="1:3">
@@ -4343,10 +4358,10 @@
         <v>534</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>795</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>796</v>
       </c>
     </row>
     <row r="33" s="1" customFormat="1" spans="1:3">
@@ -4354,10 +4369,10 @@
         <v>534</v>
       </c>
       <c r="B33" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="C33" s="1" t="s">
         <v>797</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="34" s="1" customFormat="1" spans="1:3">
@@ -4365,10 +4380,10 @@
         <v>534</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>799</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>800</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="1" spans="1:3">
@@ -4376,190 +4391,190 @@
         <v>534</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>801</v>
       </c>
-      <c r="C35" s="1" t="s">
+    </row>
+    <row r="36" s="1" customFormat="1" spans="1:3">
+      <c r="A36" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>802</v>
       </c>
-    </row>
-    <row r="36" s="2" customFormat="1"/>
-    <row r="37" s="1" customFormat="1" spans="1:3">
-      <c r="A37" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="B37" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>803</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>804</v>
-      </c>
-    </row>
+    </row>
+    <row r="37" s="2" customFormat="1"/>
     <row r="38" s="1" customFormat="1" spans="1:3">
       <c r="A38" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="39" s="1" customFormat="1" spans="1:3">
+      <c r="A39" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>803</v>
-      </c>
-      <c r="C38" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>804</v>
       </c>
-    </row>
-    <row r="39" s="3" customFormat="1" spans="1:3">
-      <c r="A39" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="B39" s="3" t="s">
+      <c r="C39" s="1" t="s">
         <v>805</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="40" s="3" customFormat="1" spans="1:3">
       <c r="A40" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>806</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="41" s="3" customFormat="1" spans="1:3">
+      <c r="A41" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B41" s="3" t="s">
+        <v>806</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>805</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="41" s="1" customFormat="1" spans="1:3">
-      <c r="A41" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>806</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="42" s="1" customFormat="1" spans="1:3">
       <c r="A42" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="43" s="1" customFormat="1" spans="1:3">
+      <c r="A43" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>806</v>
-      </c>
-      <c r="C42" s="1" t="s">
+      <c r="B43" s="1" t="s">
         <v>807</v>
       </c>
-    </row>
-    <row r="43" s="3" customFormat="1" spans="1:3">
-      <c r="A43" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="B43" s="3" t="s">
+      <c r="C43" s="1" t="s">
         <v>808</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>807</v>
       </c>
     </row>
     <row r="44" s="3" customFormat="1" spans="1:3">
       <c r="A44" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="45" s="3" customFormat="1" spans="1:3">
+      <c r="A45" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B45" s="3" t="s">
+        <v>809</v>
+      </c>
+      <c r="C45" s="3" t="s">
         <v>808</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="45" s="1" customFormat="1" spans="1:3">
-      <c r="A45" s="1" t="s">
+    </row>
+    <row r="46" s="1" customFormat="1" spans="1:3">
+      <c r="A46" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>809</v>
-      </c>
-      <c r="C45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>810</v>
       </c>
-    </row>
-    <row r="46" s="3" customFormat="1" spans="1:3">
-      <c r="A46" s="1" t="s">
-        <v>531</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>809</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>810</v>
+      <c r="C46" s="1" t="s">
+        <v>811</v>
       </c>
     </row>
     <row r="47" s="3" customFormat="1" spans="1:3">
       <c r="A47" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>810</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>811</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="48" s="3" customFormat="1" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>812</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>811</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="49" s="3" customFormat="1" spans="1:3">
       <c r="A49" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>812</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
     </row>
     <row r="50" s="3" customFormat="1" spans="1:3">
       <c r="A50" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="51" s="3" customFormat="1" spans="1:3">
+      <c r="A51" s="1" t="s">
         <v>531</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>812</v>
-      </c>
-      <c r="C50" s="3" t="s">
+      <c r="B51" s="3" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="52" s="1" customFormat="1" spans="1:4">
-      <c r="A52" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="B52" s="1" t="s">
+      <c r="C51" s="3" t="s">
         <v>814</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>788</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="53" s="1" customFormat="1" spans="1:3">
+    </row>
+    <row r="53" s="1" customFormat="1" spans="1:4">
       <c r="A53" s="1" t="s">
         <v>406</v>
       </c>
       <c r="B53" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>816</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>784</v>
       </c>
     </row>
     <row r="54" s="1" customFormat="1" spans="1:3">
@@ -4570,7 +4585,7 @@
         <v>817</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="55" s="1" customFormat="1" spans="1:3">
@@ -4581,7 +4596,7 @@
         <v>818</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>819</v>
+        <v>787</v>
       </c>
     </row>
     <row r="56" s="1" customFormat="1" spans="1:3">
@@ -4589,10 +4604,10 @@
         <v>406</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>820</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="57" s="1" customFormat="1" spans="1:3">
@@ -4600,10 +4615,10 @@
         <v>406</v>
       </c>
       <c r="B57" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="C57" s="1" t="s">
         <v>822</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="58" s="1" customFormat="1" spans="1:3">
@@ -4611,10 +4626,10 @@
         <v>406</v>
       </c>
       <c r="B58" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="C58" s="1" t="s">
         <v>824</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="59" s="1" customFormat="1" spans="1:3">
@@ -4622,10 +4637,10 @@
         <v>406</v>
       </c>
       <c r="B59" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>826</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="60" s="1" customFormat="1" spans="1:3">
@@ -4633,10 +4648,10 @@
         <v>406</v>
       </c>
       <c r="B60" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>828</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>829</v>
       </c>
     </row>
     <row r="61" s="1" customFormat="1" spans="1:3">
@@ -4644,10 +4659,10 @@
         <v>406</v>
       </c>
       <c r="B61" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="C61" s="1" t="s">
         <v>830</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="1" spans="1:3">
@@ -4655,10 +4670,10 @@
         <v>406</v>
       </c>
       <c r="B62" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="C62" s="1" t="s">
         <v>832</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>833</v>
       </c>
     </row>
     <row r="63" s="1" customFormat="1" spans="1:3">
@@ -4666,10 +4681,10 @@
         <v>406</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="C63" s="1" t="s">
         <v>834</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>835</v>
       </c>
     </row>
     <row r="64" s="1" customFormat="1" spans="1:3">
@@ -4677,10 +4692,10 @@
         <v>406</v>
       </c>
       <c r="B64" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>836</v>
-      </c>
-      <c r="C64" s="1" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="65" s="1" customFormat="1" spans="1:3">
@@ -4688,10 +4703,10 @@
         <v>406</v>
       </c>
       <c r="B65" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="C65" s="1" t="s">
         <v>838</v>
-      </c>
-      <c r="C65" s="1" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="66" s="1" customFormat="1" spans="1:3">
@@ -4699,10 +4714,10 @@
         <v>406</v>
       </c>
       <c r="B66" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="C66" s="1" t="s">
         <v>840</v>
-      </c>
-      <c r="C66" s="1" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="1" spans="1:3">
@@ -4710,10 +4725,10 @@
         <v>406</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="C67" s="1" t="s">
         <v>842</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>843</v>
       </c>
     </row>
     <row r="68" s="1" customFormat="1" spans="1:3">
@@ -4721,10 +4736,10 @@
         <v>406</v>
       </c>
       <c r="B68" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="C68" s="1" t="s">
         <v>844</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="69" s="1" customFormat="1" spans="1:3">
@@ -4732,33 +4747,33 @@
         <v>406</v>
       </c>
       <c r="B69" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="C69" s="1" t="s">
         <v>846</v>
       </c>
-      <c r="C69" s="1" t="s">
+    </row>
+    <row r="70" s="1" customFormat="1" spans="1:3">
+      <c r="A70" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B70" s="1" t="s">
         <v>847</v>
       </c>
-    </row>
-    <row r="70" s="1" customFormat="1"/>
-    <row r="71" s="1" customFormat="1" spans="1:3">
-      <c r="A71" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>814</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>788</v>
-      </c>
-    </row>
+      <c r="C70" s="1" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="71" s="1" customFormat="1"/>
     <row r="72" s="1" customFormat="1" spans="1:3">
       <c r="A72" s="1" t="s">
         <v>520</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>784</v>
+        <v>789</v>
       </c>
     </row>
     <row r="73" s="1" customFormat="1" spans="1:3">
@@ -4769,7 +4784,7 @@
         <v>817</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
     </row>
     <row r="74" s="1" customFormat="1" spans="1:3">
@@ -4780,7 +4795,7 @@
         <v>818</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>819</v>
+        <v>787</v>
       </c>
     </row>
     <row r="75" s="1" customFormat="1" spans="1:3">
@@ -4788,10 +4803,10 @@
         <v>520</v>
       </c>
       <c r="B75" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="C75" s="1" t="s">
         <v>820</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="76" s="1" customFormat="1" spans="1:3">
@@ -4799,10 +4814,10 @@
         <v>520</v>
       </c>
       <c r="B76" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="C76" s="1" t="s">
         <v>822</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>823</v>
       </c>
     </row>
     <row r="77" s="1" customFormat="1" spans="1:3">
@@ -4810,10 +4825,10 @@
         <v>520</v>
       </c>
       <c r="B77" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="C77" s="1" t="s">
         <v>824</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>825</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="1" spans="1:3">
@@ -4821,10 +4836,10 @@
         <v>520</v>
       </c>
       <c r="B78" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="C78" s="1" t="s">
         <v>826</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="79" s="1" customFormat="1" spans="1:3">
@@ -4832,10 +4847,10 @@
         <v>520</v>
       </c>
       <c r="B79" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="C79" s="1" t="s">
         <v>828</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>829</v>
       </c>
     </row>
     <row r="80" s="1" customFormat="1" spans="1:3">
@@ -4843,10 +4858,10 @@
         <v>520</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>848</v>
+        <v>829</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>849</v>
+        <v>830</v>
       </c>
     </row>
     <row r="81" s="1" customFormat="1" spans="1:3">
@@ -4854,10 +4869,10 @@
         <v>520</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>830</v>
+        <v>849</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>831</v>
+        <v>850</v>
       </c>
     </row>
     <row r="82" s="1" customFormat="1" spans="1:3">
@@ -4865,10 +4880,10 @@
         <v>520</v>
       </c>
       <c r="B82" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="C82" s="1" t="s">
         <v>832</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>833</v>
       </c>
     </row>
     <row r="83" s="1" customFormat="1" spans="1:3">
@@ -4876,10 +4891,10 @@
         <v>520</v>
       </c>
       <c r="B83" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="C83" s="1" t="s">
         <v>834</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>835</v>
       </c>
     </row>
     <row r="84" s="1" customFormat="1" spans="1:3">
@@ -4887,10 +4902,10 @@
         <v>520</v>
       </c>
       <c r="B84" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="C84" s="1" t="s">
         <v>836</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>837</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="1" spans="1:3">
@@ -4898,10 +4913,10 @@
         <v>520</v>
       </c>
       <c r="B85" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="C85" s="1" t="s">
         <v>838</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>839</v>
       </c>
     </row>
     <row r="86" s="1" customFormat="1" spans="1:3">
@@ -4909,10 +4924,10 @@
         <v>520</v>
       </c>
       <c r="B86" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>840</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="87" s="1" customFormat="1" spans="1:3">
@@ -4920,10 +4935,10 @@
         <v>520</v>
       </c>
       <c r="B87" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>842</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>843</v>
       </c>
     </row>
     <row r="88" s="1" customFormat="1" spans="1:3">
@@ -4931,10 +4946,10 @@
         <v>520</v>
       </c>
       <c r="B88" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>844</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>845</v>
       </c>
     </row>
     <row r="89" s="1" customFormat="1" spans="1:3">
@@ -4942,36 +4957,36 @@
         <v>520</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>846</v>
       </c>
-      <c r="C89" s="1" t="s">
+    </row>
+    <row r="90" s="1" customFormat="1" spans="1:3">
+      <c r="A90" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B90" s="1" t="s">
         <v>847</v>
       </c>
-    </row>
-    <row r="90" s="1" customFormat="1"/>
-    <row r="91" s="1" customFormat="1" spans="1:4">
-      <c r="A91" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="B91" s="1" t="s">
-        <v>850</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>851</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>852</v>
-      </c>
-    </row>
-    <row r="92" s="1" customFormat="1" spans="1:3">
+      <c r="C90" s="1" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="91" s="1" customFormat="1"/>
+    <row r="92" s="1" customFormat="1" spans="1:4">
       <c r="A92" s="1" t="s">
         <v>406</v>
       </c>
       <c r="B92" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="D92" s="1" t="s">
         <v>853</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>854</v>
       </c>
     </row>
     <row r="93" s="1" customFormat="1" spans="1:3">
@@ -4979,10 +4994,10 @@
         <v>406</v>
       </c>
       <c r="B93" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="C93" s="1" t="s">
         <v>855</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="94" s="1" customFormat="1" spans="1:3">
@@ -4990,10 +5005,10 @@
         <v>406</v>
       </c>
       <c r="B94" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="C94" s="1" t="s">
         <v>857</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="95" s="1" customFormat="1" spans="1:3">
@@ -5004,7 +5019,7 @@
         <v>858</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="96" s="1" customFormat="1" spans="1:3">
@@ -5015,7 +5030,7 @@
         <v>859</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
     </row>
     <row r="97" s="1" customFormat="1" spans="1:3">
@@ -5026,7 +5041,7 @@
         <v>860</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="98" s="1" customFormat="1" spans="1:3">
@@ -5037,7 +5052,7 @@
         <v>861</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="99" s="1" customFormat="1" spans="1:3">
@@ -5048,7 +5063,7 @@
         <v>862</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>849</v>
+        <v>830</v>
       </c>
     </row>
     <row r="100" s="1" customFormat="1" spans="1:3">
@@ -5059,7 +5074,7 @@
         <v>863</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>831</v>
+        <v>850</v>
       </c>
     </row>
     <row r="101" s="1" customFormat="1" spans="1:3">
@@ -5070,7 +5085,7 @@
         <v>864</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="102" s="1" customFormat="1" spans="1:3">
@@ -5081,7 +5096,7 @@
         <v>865</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="103" s="1" customFormat="1" spans="1:3">
@@ -5092,7 +5107,7 @@
         <v>866</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="104" s="1" customFormat="1" spans="1:3">
@@ -5103,7 +5118,7 @@
         <v>867</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="105" s="1" customFormat="1" spans="1:3">
@@ -5114,7 +5129,7 @@
         <v>868</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="106" s="1" customFormat="1" spans="1:3">
@@ -5125,7 +5140,7 @@
         <v>869</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="107" s="1" customFormat="1" spans="1:3">
@@ -5136,7 +5151,7 @@
         <v>870</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="108" s="1" customFormat="1" spans="1:3">
@@ -5147,30 +5162,30 @@
         <v>871</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="109" s="1" customFormat="1"/>
-    <row r="110" s="1" customFormat="1" spans="1:3">
-      <c r="A110" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="B110" s="1" t="s">
-        <v>822</v>
-      </c>
-      <c r="C110" s="1" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="109" s="1" customFormat="1" spans="1:3">
+      <c r="A109" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="B109" s="1" t="s">
         <v>872</v>
       </c>
-    </row>
+      <c r="C109" s="1" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="110" s="1" customFormat="1"/>
     <row r="111" s="1" customFormat="1" spans="1:3">
       <c r="A111" s="1" t="s">
         <v>520</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>850</v>
+        <v>823</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>851</v>
+        <v>873</v>
       </c>
     </row>
     <row r="112" s="1" customFormat="1" spans="1:3">
@@ -5178,10 +5193,10 @@
         <v>520</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="113" s="1" customFormat="1" spans="1:3">
@@ -5189,10 +5204,10 @@
         <v>520</v>
       </c>
       <c r="B113" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>855</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="114" s="1" customFormat="1" spans="1:3">
@@ -5200,10 +5215,10 @@
         <v>520</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="C114" s="1" t="s">
         <v>857</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>819</v>
       </c>
     </row>
     <row r="115" s="1" customFormat="1" spans="1:3">
@@ -5214,7 +5229,7 @@
         <v>858</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
     </row>
     <row r="116" s="1" customFormat="1" spans="1:3">
@@ -5222,10 +5237,10 @@
         <v>520</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>822</v>
-      </c>
-      <c r="C116" s="1" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="117" s="1" customFormat="1" spans="1:3">
@@ -5233,10 +5248,10 @@
         <v>520</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>859</v>
+        <v>823</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>825</v>
+        <v>873</v>
       </c>
     </row>
     <row r="118" s="1" customFormat="1" spans="1:3">
@@ -5247,7 +5262,7 @@
         <v>860</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="119" s="1" customFormat="1" spans="1:3">
@@ -5258,7 +5273,7 @@
         <v>861</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
     </row>
     <row r="120" s="1" customFormat="1" spans="1:3">
@@ -5269,7 +5284,7 @@
         <v>862</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>849</v>
+        <v>830</v>
       </c>
     </row>
     <row r="121" s="1" customFormat="1" spans="1:3">
@@ -5280,7 +5295,7 @@
         <v>863</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>831</v>
+        <v>850</v>
       </c>
     </row>
     <row r="122" s="1" customFormat="1" spans="1:3">
@@ -5291,7 +5306,7 @@
         <v>864</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
     </row>
     <row r="123" s="1" customFormat="1" spans="1:3">
@@ -5302,7 +5317,7 @@
         <v>865</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
     </row>
     <row r="124" s="1" customFormat="1" spans="1:3">
@@ -5313,7 +5328,7 @@
         <v>866</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
     </row>
     <row r="125" s="1" customFormat="1" spans="1:3">
@@ -5324,7 +5339,7 @@
         <v>867</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
     </row>
     <row r="126" s="1" customFormat="1" spans="1:3">
@@ -5335,7 +5350,7 @@
         <v>868</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
     </row>
     <row r="127" s="1" customFormat="1" spans="1:3">
@@ -5346,7 +5361,7 @@
         <v>869</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
     </row>
     <row r="128" s="1" customFormat="1" spans="1:3">
@@ -5357,7 +5372,7 @@
         <v>870</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
     </row>
     <row r="129" s="1" customFormat="1" spans="1:3">
@@ -5368,32 +5383,32 @@
         <v>871</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>847</v>
-      </c>
-    </row>
-    <row r="131" s="1" customFormat="1" spans="1:4">
-      <c r="A131" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="B131" s="1" t="s">
-        <v>873</v>
-      </c>
-      <c r="C131" s="1" t="s">
-        <v>790</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>874</v>
-      </c>
-    </row>
-    <row r="132" s="1" customFormat="1" spans="1:3">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="130" s="1" customFormat="1" spans="1:3">
+      <c r="A130" s="1" t="s">
+        <v>520</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="132" s="1" customFormat="1" spans="1:4">
       <c r="A132" s="1" t="s">
         <v>534</v>
       </c>
       <c r="B132" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>791</v>
+      </c>
+      <c r="D132" s="1" t="s">
         <v>875</v>
-      </c>
-      <c r="C132" s="1" t="s">
-        <v>792</v>
       </c>
     </row>
     <row r="133" s="1" customFormat="1" spans="1:3">
@@ -5404,7 +5419,7 @@
         <v>876</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
     </row>
     <row r="134" s="1" customFormat="1" spans="1:3">
@@ -5415,7 +5430,7 @@
         <v>877</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
     </row>
     <row r="135" s="1" customFormat="1" spans="1:3">
@@ -5426,7 +5441,7 @@
         <v>878</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
     </row>
     <row r="136" s="1" customFormat="1" spans="1:3">
@@ -5437,7 +5452,7 @@
         <v>879</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="137" s="1" customFormat="1" spans="1:3">
@@ -5448,18 +5463,18 @@
         <v>880</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="138" s="3" customFormat="1" spans="1:3">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="138" s="1" customFormat="1" spans="1:3">
       <c r="A138" s="1" t="s">
         <v>534</v>
       </c>
-      <c r="B138" s="3" t="s">
+      <c r="B138" s="1" t="s">
         <v>881</v>
       </c>
-      <c r="C138" s="3" t="s">
-        <v>882</v>
+      <c r="C138" s="1" t="s">
+        <v>803</v>
       </c>
     </row>
     <row r="139" s="3" customFormat="1" spans="1:3">
@@ -5467,10 +5482,10 @@
         <v>534</v>
       </c>
       <c r="B139" s="3" t="s">
+        <v>882</v>
+      </c>
+      <c r="C139" s="3" t="s">
         <v>883</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>884</v>
       </c>
     </row>
     <row r="140" s="3" customFormat="1" spans="1:3">
@@ -5478,10 +5493,10 @@
         <v>534</v>
       </c>
       <c r="B140" s="3" t="s">
+        <v>884</v>
+      </c>
+      <c r="C140" s="3" t="s">
         <v>885</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>884</v>
       </c>
     </row>
     <row r="141" s="3" customFormat="1" spans="1:3">
@@ -5492,7 +5507,7 @@
         <v>886</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="142" s="3" customFormat="1" spans="1:3">
@@ -5500,10 +5515,10 @@
         <v>534</v>
       </c>
       <c r="B142" s="3" t="s">
+        <v>887</v>
+      </c>
+      <c r="C142" s="3" t="s">
         <v>888</v>
-      </c>
-      <c r="C142" s="3" t="s">
-        <v>889</v>
       </c>
     </row>
     <row r="143" s="3" customFormat="1" spans="1:3">
@@ -5511,10 +5526,10 @@
         <v>534</v>
       </c>
       <c r="B143" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="C143" s="3" t="s">
         <v>890</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>891</v>
       </c>
     </row>
     <row r="144" s="3" customFormat="1" spans="1:3">
@@ -5522,10 +5537,10 @@
         <v>534</v>
       </c>
       <c r="B144" s="3" t="s">
+        <v>891</v>
+      </c>
+      <c r="C144" s="3" t="s">
         <v>892</v>
-      </c>
-      <c r="C144" s="3" t="s">
-        <v>891</v>
       </c>
     </row>
     <row r="145" s="3" customFormat="1" spans="1:3">
@@ -5536,7 +5551,7 @@
         <v>893</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
     </row>
     <row r="146" s="3" customFormat="1" spans="1:3">
@@ -5544,10 +5559,10 @@
         <v>534</v>
       </c>
       <c r="B146" s="3" t="s">
+        <v>894</v>
+      </c>
+      <c r="C146" s="3" t="s">
         <v>895</v>
-      </c>
-      <c r="C146" s="3" t="s">
-        <v>896</v>
       </c>
     </row>
     <row r="147" s="3" customFormat="1" spans="1:3">
@@ -5555,10 +5570,10 @@
         <v>534</v>
       </c>
       <c r="B147" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="C147" s="3" t="s">
         <v>897</v>
-      </c>
-      <c r="C147" s="3" t="s">
-        <v>898</v>
       </c>
     </row>
     <row r="148" s="3" customFormat="1" spans="1:3">
@@ -5566,10 +5581,10 @@
         <v>534</v>
       </c>
       <c r="B148" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="C148" s="3" t="s">
         <v>899</v>
-      </c>
-      <c r="C148" s="3" t="s">
-        <v>900</v>
       </c>
     </row>
     <row r="149" s="3" customFormat="1" spans="1:3">
@@ -5577,14 +5592,47 @@
         <v>534</v>
       </c>
       <c r="B149" s="3" t="s">
+        <v>900</v>
+      </c>
+      <c r="C149" s="3" t="s">
         <v>901</v>
       </c>
-      <c r="C149" s="3" t="s">
+    </row>
+    <row r="150" s="3" customFormat="1" spans="1:3">
+      <c r="A150" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="B150" s="3" t="s">
         <v>902</v>
       </c>
-    </row>
-    <row r="150" spans="1:1">
-      <c r="A150" s="5"/>
+      <c r="C150" s="3" t="s">
+        <v>903</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="5"/>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" t="s">
+        <v>377</v>
+      </c>
+      <c r="B152" t="s">
+        <v>904</v>
+      </c>
+      <c r="C152" t="s">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" t="s">
+        <v>377</v>
+      </c>
+      <c r="B153" t="s">
+        <v>906</v>
+      </c>
+      <c r="C153" t="s">
+        <v>907</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7059,9 +7107,9 @@
   <dimension ref="A1:F1044"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A328" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A350" sqref="A350"/>
+      <selection pane="bottomLeft" activeCell="A179" sqref="A179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="5"/>

</xml_diff>

<commit_message>
Add area renaming for bfa/cmr/cod/cog/gin/gmb/gnb/ken/lso/mli/moz/nga/sle/ssd/tgo_survey
</commit_message>
<xml_diff>
--- a/data/hivdata_survey_datasets.xlsx
+++ b/data/hivdata_survey_datasets.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11799" uniqueCount="908">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11808" uniqueCount="914">
   <si>
     <t>Tables reflect analysis ready datasets. Non-analytical values (don't know, missing) are recoded as NA.</t>
   </si>
@@ -2808,6 +2808,24 @@
   </si>
   <si>
     <t>Bururi</t>
+  </si>
+  <si>
+    <t>Hauts-Bassins</t>
+  </si>
+  <si>
+    <t>Hauts Bassins</t>
+  </si>
+  <si>
+    <t>Cascade</t>
+  </si>
+  <si>
+    <t>Cascades</t>
+  </si>
+  <si>
+    <t>Plateau-Central</t>
+  </si>
+  <si>
+    <t>Plateau Central</t>
   </si>
 </sst>
 </file>
@@ -3969,12 +3987,12 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D153"/>
+  <dimension ref="A1:D157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="$A21:$XFD21"/>
+      <selection pane="bottomLeft" activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="3"/>
@@ -5632,6 +5650,39 @@
       </c>
       <c r="C153" t="s">
         <v>907</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" t="s">
+        <v>381</v>
+      </c>
+      <c r="B155" t="s">
+        <v>908</v>
+      </c>
+      <c r="C155" t="s">
+        <v>909</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" t="s">
+        <v>381</v>
+      </c>
+      <c r="B156" t="s">
+        <v>910</v>
+      </c>
+      <c r="C156" t="s">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" t="s">
+        <v>381</v>
+      </c>
+      <c r="B157" t="s">
+        <v>912</v>
+      </c>
+      <c r="C157" t="s">
+        <v>913</v>
       </c>
     </row>
   </sheetData>
@@ -7107,9 +7158,9 @@
   <dimension ref="A1:F1044"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A326" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A179" sqref="A179"/>
+      <selection pane="bottomLeft" activeCell="A353" sqref="A353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" outlineLevelCol="5"/>

</xml_diff>